<commit_message>
changes in opportunity page and opportunity test
</commit_message>
<xml_diff>
--- a/src/main/java/testData/OpportunityTestData.xlsx
+++ b/src/main/java/testData/OpportunityTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26DA4CE7-A7E2-493C-9D0F-D3479E3932D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2946572F-2978-4A45-9B67-60A216DF18A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Opportunity Name</t>
   </si>
@@ -57,6 +57,9 @@
     <t>Probability</t>
   </si>
   <si>
+    <t>Lead</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -75,6 +78,9 @@
     <t>Prospecting</t>
   </si>
   <si>
+    <t>Regina</t>
+  </si>
+  <si>
     <t>New opportunity from campaign</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
   </si>
   <si>
     <t>Qualification</t>
+  </si>
+  <si>
+    <t>LeadMandatory</t>
   </si>
   <si>
     <t>Renewal for key account</t>
@@ -97,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +121,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,12 +150,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,10 +509,11 @@
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,66 +538,75 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>5000</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>45874</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" ht="28.5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>12000</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2">
         <v>45879</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
-        <v>19</v>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in Create Opportunity
</commit_message>
<xml_diff>
--- a/src/main/java/testData/OpportunityTestData.xlsx
+++ b/src/main/java/testData/OpportunityTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2946572F-2978-4A45-9B67-60A216DF18A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5F6EA7A-4462-4CC7-B7CA-52667FBEBF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Opportunity Name</t>
   </si>
@@ -63,7 +63,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>AutoOpp</t>
+    <t>AutoOppabc</t>
   </si>
   <si>
     <t>New Business</t>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>New opportunity from campaign</t>
+  </si>
+  <si>
+    <t>AutoOppxyz</t>
   </si>
   <si>
     <t>Existing</t>
@@ -497,7 +500,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -579,34 +582,34 @@
     </row>
     <row r="3" spans="1:10" ht="28.5">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>12000</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2">
         <v>45879</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4">
         <v>30</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Opportunity test and opportunity page
</commit_message>
<xml_diff>
--- a/src/main/java/testData/OpportunityTestData.xlsx
+++ b/src/main/java/testData/OpportunityTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5F6EA7A-4462-4CC7-B7CA-52667FBEBF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1877805-CA38-4276-B17B-41A094482F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Opportunity Name</t>
   </si>
@@ -103,13 +103,64 @@
   </si>
   <si>
     <t>Renewal for key account</t>
+  </si>
+  <si>
+    <t>AutoOppProbBlank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Business	</t>
+  </si>
+  <si>
+    <t>Call customer</t>
+  </si>
+  <si>
+    <t>qualification</t>
+  </si>
+  <si>
+    <t>AutoOppmnt</t>
+  </si>
+  <si>
+    <t>Joe Biden</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>AutoOpptemp</t>
+  </si>
+  <si>
+    <t>Mahesh Patel</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>AutoOpptemper</t>
+  </si>
+  <si>
+    <t>Lily</t>
+  </si>
+  <si>
+    <t>AutoOppfifa</t>
+  </si>
+  <si>
+    <t>sumit</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>AutoOppTst</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +181,12 @@
       <color rgb="FF212529"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -153,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -161,6 +218,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -497,17 +558,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
@@ -612,6 +673,188 @@
         <v>23</v>
       </c>
     </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.25">
+      <c r="B5">
+        <v>6000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2">
+        <v>45936</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="29.25">
+      <c r="A7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>10000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2">
+        <v>45879</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>2000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2">
+        <v>46013</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="4">
+        <v>30</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>3000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>89990</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2">
+        <v>45886</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove conflicts in basepage
</commit_message>
<xml_diff>
--- a/src/main/java/testData/OpportunityTestData.xlsx
+++ b/src/main/java/testData/OpportunityTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26DA4CE7-A7E2-493C-9D0F-D3479E3932D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2946572F-2978-4A45-9B67-60A216DF18A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Opportunity Name</t>
   </si>
@@ -57,6 +57,9 @@
     <t>Probability</t>
   </si>
   <si>
+    <t>Lead</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -75,6 +78,9 @@
     <t>Prospecting</t>
   </si>
   <si>
+    <t>Regina</t>
+  </si>
+  <si>
     <t>New opportunity from campaign</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
   </si>
   <si>
     <t>Qualification</t>
+  </si>
+  <si>
+    <t>LeadMandatory</t>
   </si>
   <si>
     <t>Renewal for key account</t>
@@ -97,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +121,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,12 +150,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,10 +509,11 @@
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,66 +538,75 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>5000</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>45874</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" ht="28.5">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>12000</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2">
         <v>45879</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4">
         <v>30</v>
       </c>
-      <c r="I3" t="s">
-        <v>19</v>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>